<commit_message>
Changed a bit here and there
</commit_message>
<xml_diff>
--- a/iphone-dates-2019.xlsx
+++ b/iphone-dates-2019.xlsx
@@ -1,30 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ratman\PycharmProjects\pandas-apple-stock\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bratiu/PycharmProjects/pandas-apple-stock/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EDFA4E9-6C9C-8E4C-8F50-9A059B2329E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22992" windowHeight="9168"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>iPhone XS, XS Max</t>
   </si>
@@ -84,13 +95,19 @@
   </si>
   <si>
     <t>tem2</t>
+  </si>
+  <si>
+    <t>Iphone 12</t>
+  </si>
+  <si>
+    <t>Iphone 13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,7 +116,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -119,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -142,40 +166,21 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFEEEEEE"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFEEEEEE"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFEEEEEE"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF111111"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,271 +460,303 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.5546875" style="5" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="40.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="4">
         <v>2018</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="5">
         <v>43729</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="3">
         <f>DATE(YEAR(C2)-2019+B2, MONTH(C2), DAY(C2))</f>
         <v>43364</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="4">
         <v>2018</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="5">
         <v>43764</v>
       </c>
-      <c r="D3" s="5">
-        <f t="shared" ref="D3:D17" si="0">DATE(YEAR(C3)-2019+B3, MONTH(C3), DAY(C3))</f>
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D19" si="0">DATE(YEAR(C3)-2019+B3, MONTH(C3), DAY(C3))</f>
         <v>43399</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <v>2017</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>43772</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="3">
         <f t="shared" si="0"/>
         <v>43042</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="4">
         <v>2016</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>43555</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="3">
         <f t="shared" si="0"/>
         <v>42460</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="4">
         <v>2017</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="5">
         <v>43730</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="3">
         <f t="shared" si="0"/>
         <v>43000</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="4">
         <v>2016</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="5">
         <v>43724</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="3">
         <f t="shared" si="0"/>
         <v>42629</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="4">
         <v>2015</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="5">
         <v>43728</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="3">
         <f t="shared" si="0"/>
         <v>42267</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="4">
         <v>2014</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="5">
         <v>43728</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>41902</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="4">
         <v>2013</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="5">
         <v>43718</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="3">
         <f t="shared" si="0"/>
         <v>41527</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+    <row r="11" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="4">
         <v>2012</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="5">
         <v>43729</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="3">
         <f t="shared" si="0"/>
         <v>41173</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="4">
         <v>2011</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="5">
         <v>43752</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
         <v>40830</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="4">
         <v>2010</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="5">
         <v>43637</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
         <v>40350</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="4">
         <v>2009</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="5">
         <v>43635</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="3">
         <f t="shared" si="0"/>
         <v>39983</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
+    <row r="15" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="4">
         <v>2008</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="5">
         <v>43645</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="3">
         <f t="shared" si="0"/>
         <v>39628</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="4">
         <v>2019</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="5">
         <v>43728</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="3">
         <f t="shared" si="0"/>
         <v>43728</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+    <row r="17" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="4">
         <v>2007</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="5">
         <v>43720</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="3">
         <f t="shared" si="0"/>
         <v>39337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="4">
+        <v>2020</v>
+      </c>
+      <c r="C18" s="5">
+        <v>44857</v>
+      </c>
+      <c r="D18" s="3">
+        <f>DATE(B18, MONTH(C18), DAY(C18))</f>
+        <v>44127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="4">
+        <v>2021</v>
+      </c>
+      <c r="C19" s="5">
+        <v>44828</v>
+      </c>
+      <c r="D19" s="3">
+        <f>DATE(B19, MONTH(C19), DAY(C19))</f>
+        <v>44463</v>
       </c>
     </row>
   </sheetData>

</xml_diff>